<commit_message>
Fixing Lab 3 charts
</commit_message>
<xml_diff>
--- a/03_ficks_principle/03_ficks_principle_data.xlsx
+++ b/03_ficks_principle/03_ficks_principle_data.xlsx
@@ -158,45 +158,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -500,7 +472,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -559,7 +531,7 @@
       <c r="E3" s="4">
         <v>0.15</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="5">
@@ -580,7 +552,7 @@
       <c r="E4" s="4">
         <v>231</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="5">
@@ -601,7 +573,7 @@
       <c r="E5" s="4">
         <v>5500</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="5">
@@ -622,7 +594,7 @@
       <c r="E6" s="4">
         <v>5468</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="5">
@@ -632,11 +604,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H6">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>